<commit_message>
version 1.0.0.8: support us delay
</commit_message>
<xml_diff>
--- a/Script Grammer Notes.xlsx
+++ b/Script Grammer Notes.xlsx
@@ -55,9 +55,6 @@
     <t>delay</t>
   </si>
   <si>
-    <t>delay 50 ms</t>
-  </si>
-  <si>
     <t>Statement</t>
   </si>
   <si>
@@ -2643,6 +2640,9 @@
   </si>
   <si>
     <t>Grammar Notes</t>
+  </si>
+  <si>
+    <t>delay 5000 us (5ms)</t>
   </si>
 </sst>
 </file>
@@ -3165,7 +3165,7 @@
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3177,20 +3177,20 @@
   <sheetData>
     <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3205,30 +3205,30 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="22"/>
       <c r="B5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="24"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="22"/>
       <c r="B6" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="24"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="22"/>
       <c r="B7" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="24"/>
     </row>
@@ -3237,28 +3237,28 @@
         <v>3</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="24"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="24"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="24"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="24"/>
     </row>
@@ -3267,10 +3267,10 @@
         <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -3278,10 +3278,10 @@
         <v>4</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -3289,10 +3289,10 @@
         <v>5</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -3300,72 +3300,72 @@
         <v>10</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>11</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="15" t="s">
-        <v>55</v>
-      </c>
       <c r="C17" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="26"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" s="26"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="26"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" s="26"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C22" s="26"/>
     </row>
@@ -3374,37 +3374,37 @@
         <v>6</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C23" s="26"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" s="26"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C25" s="27"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -3419,10 +3419,10 @@
         <v>8</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -3430,125 +3430,125 @@
         <v>9</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
     </row>
     <row r="34" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A34" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B36" s="21"/>
       <c r="C36" s="21"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C37" s="5"/>
     </row>
     <row r="38" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="22"/>
       <c r="B40" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -3587,32 +3587,32 @@
   <sheetData>
     <row r="1" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B1" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.3">
@@ -3620,32 +3620,32 @@
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B8" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B9" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B11" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B12" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B13" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.3">
@@ -3653,27 +3653,27 @@
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B15" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B16" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
@@ -3681,32 +3681,32 @@
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B24" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.3">
@@ -3714,57 +3714,57 @@
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" s="18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.3">

</xml_diff>